<commit_message>
Implemented saving to bronv3
</commit_message>
<xml_diff>
--- a/pybron/rws_bron/data/Mapping en definitie BRO GMW.xlsx
+++ b/pybron/rws_bron/data/Mapping en definitie BRO GMW.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\RWS Ketentest\basis-python-project\rws_ketentest\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\RWS Ketentest\basis-python-project\rws_bron\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BE52A5-661D-40F0-8AF9-16885E84525C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81650B4E-461C-4D86-B63C-183160705870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="320">
   <si>
     <t xml:space="preserve">RegistrationObject </t>
   </si>
@@ -982,6 +982,12 @@
   </si>
   <si>
     <t>sedSumpLength</t>
+  </si>
+  <si>
+    <t>[GldBroID]</t>
+  </si>
+  <si>
+    <t>GLDBROID</t>
   </si>
 </sst>
 </file>
@@ -1416,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q75" sqref="Q75"/>
+    <sheetView tabSelected="1" topLeftCell="F54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P86" sqref="P86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5526,13 +5532,13 @@
         <v>129</v>
       </c>
       <c r="P86" t="s">
-        <v>297</v>
+        <v>319</v>
       </c>
       <c r="Q86" t="s">
         <v>297</v>
       </c>
       <c r="R86" t="s">
-        <v>113</v>
+        <v>318</v>
       </c>
       <c r="S86" t="s">
         <v>85</v>

</xml_diff>